<commit_message>
added building list, more cart functionality
</commit_message>
<xml_diff>
--- a/ustore_inventory.xlsx
+++ b/ustore_inventory.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11013"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11110"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/gregsmith/Desktop/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/gregsmith/Desktop/tigertask/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{843C2226-6754-B147-8883-B1DBF0095DA7}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2584BFAA-475F-5E44-9823-3F0318FE47CB}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="380" yWindow="460" windowWidth="28040" windowHeight="16120" xr2:uid="{3B85A2FB-0F4E-714C-ACD8-957C335DFFB0}"/>
   </bookViews>
@@ -438,9 +438,6 @@
     <t>SOLO Party Cups, Orange (36ct)</t>
   </si>
   <si>
-    <t>School Supplies</t>
-  </si>
-  <si>
     <t>TopFlight Princeton Folder</t>
   </si>
   <si>
@@ -490,6 +487,9 @@
   </si>
   <si>
     <t>Desk-Style Hi-Liter (2pc)</t>
+  </si>
+  <si>
+    <t>School</t>
   </si>
 </sst>
 </file>
@@ -852,8 +852,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F4EC96C8-0B8D-2B4D-B1F3-C4B03D42A84B}">
   <dimension ref="A1:C145"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D123" sqref="D123"/>
+    <sheetView tabSelected="1" topLeftCell="A119" workbookViewId="0">
+      <selection activeCell="C137" sqref="C137"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -2273,189 +2273,189 @@
     </row>
     <row r="129" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A129" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="B129">
         <v>2.5</v>
       </c>
       <c r="C129" t="s">
-        <v>135</v>
+        <v>152</v>
       </c>
     </row>
     <row r="130" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A130" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="B130">
         <v>5</v>
       </c>
       <c r="C130" t="s">
-        <v>135</v>
+        <v>152</v>
       </c>
     </row>
     <row r="131" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A131" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
       <c r="B131">
         <v>3</v>
       </c>
       <c r="C131" t="s">
-        <v>135</v>
+        <v>152</v>
       </c>
     </row>
     <row r="132" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A132" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
       <c r="B132">
         <v>3</v>
       </c>
       <c r="C132" t="s">
-        <v>135</v>
+        <v>152</v>
       </c>
     </row>
     <row r="133" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A133" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="B133">
         <v>4</v>
       </c>
       <c r="C133" t="s">
-        <v>135</v>
+        <v>152</v>
       </c>
     </row>
     <row r="134" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A134" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="B134">
         <v>8</v>
       </c>
       <c r="C134" t="s">
-        <v>135</v>
+        <v>152</v>
       </c>
     </row>
     <row r="135" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A135" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="B135">
         <v>10</v>
       </c>
       <c r="C135" t="s">
-        <v>135</v>
+        <v>152</v>
       </c>
     </row>
     <row r="136" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A136" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="B136">
         <v>6</v>
       </c>
       <c r="C136" t="s">
-        <v>135</v>
+        <v>152</v>
       </c>
     </row>
     <row r="137" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A137" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
       <c r="B137">
         <v>4</v>
       </c>
       <c r="C137" t="s">
-        <v>135</v>
+        <v>152</v>
       </c>
     </row>
     <row r="138" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A138" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
       <c r="B138">
         <v>2.5</v>
       </c>
       <c r="C138" t="s">
-        <v>135</v>
+        <v>152</v>
       </c>
     </row>
     <row r="139" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A139" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
       <c r="B139">
         <v>3</v>
       </c>
       <c r="C139" t="s">
-        <v>135</v>
+        <v>152</v>
       </c>
     </row>
     <row r="140" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A140" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
       <c r="B140">
         <v>35</v>
       </c>
       <c r="C140" t="s">
-        <v>135</v>
+        <v>152</v>
       </c>
     </row>
     <row r="141" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A141" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
       <c r="B141">
         <v>3</v>
       </c>
       <c r="C141" t="s">
-        <v>135</v>
+        <v>152</v>
       </c>
     </row>
     <row r="142" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A142" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
       <c r="B142">
         <v>3</v>
       </c>
       <c r="C142" t="s">
-        <v>135</v>
+        <v>152</v>
       </c>
     </row>
     <row r="143" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A143" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
       <c r="B143">
         <v>3</v>
       </c>
       <c r="C143" t="s">
-        <v>135</v>
+        <v>152</v>
       </c>
     </row>
     <row r="144" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A144" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
       <c r="B144">
         <v>2.5</v>
       </c>
       <c r="C144" t="s">
-        <v>135</v>
+        <v>152</v>
       </c>
     </row>
     <row r="145" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A145" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
       <c r="B145">
         <v>2</v>
       </c>
       <c r="C145" t="s">
-        <v>135</v>
+        <v>152</v>
       </c>
     </row>
   </sheetData>

</xml_diff>